<commit_message>
v1.1 update Owner Status
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_Publish_Upload_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_Publish_Upload_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F390A6-D0A3-42A8-9C9D-C4C47A2F3BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_PUBLISH&amp;UPLOAD_REVIEWS" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,9 +99,6 @@
     <t>Ahmed abouzid</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>TC-PUB-007 &amp; TC-PUB-008</t>
   </si>
   <si>
@@ -125,12 +121,15 @@
   </si>
   <si>
     <t>Initial version</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -608,30 +607,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="6"/>
+    <tableColumn id="1" name="Date" dataDxfId="15"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="0">
+    <tableColumn id="1" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -935,29 +934,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="D1" zoomScale="50" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="45.5546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="115.6640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="103.44140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="37.44140625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="1" max="1" width="16.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="115.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="103.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -989,7 +988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="63" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="63" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>45768</v>
       </c>
@@ -1015,11 +1014,11 @@
         <v>20</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="J2" s="12"/>
     </row>
-    <row r="3" spans="1:10" ht="63" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="63" x14ac:dyDescent="0.35">
       <c r="A3" s="11">
         <v>45768</v>
       </c>
@@ -1027,7 +1026,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>14</v>
@@ -1036,28 +1035,28 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="63" x14ac:dyDescent="0.35">
       <c r="A4" s="11">
         <v>45768</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>14</v>
@@ -1066,20 +1065,20 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="J4" s="12"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1091,7 +1090,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1103,7 +1102,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1115,7 +1114,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1127,7 +1126,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1139,7 +1138,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1151,7 +1150,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1163,7 +1162,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1175,22 +1174,22 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1203,22 +1202,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1232,7 +1231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1240,50 +1239,50 @@
         <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D4" si="0">DATE(2025,4,21)</f>
+        <f t="shared" ref="D2" si="0">DATE(2025,4,21)</f>
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>